<commit_message>
bug update in Kbar calculation
There was an error in the Kbar now-casting. It changes slightly some numerical data but the main results stay the same
</commit_message>
<xml_diff>
--- a/Figures/figure2.xlsx
+++ b/Figures/figure2.xlsx
@@ -485,10 +485,10 @@
         <v>47.99443885251737</v>
       </c>
       <c r="C2" t="n">
-        <v>89.45955656993578</v>
+        <v>81.09106943735266</v>
       </c>
       <c r="D2" t="n">
-        <v>18.508453305825</v>
+        <v>10.13996617324147</v>
       </c>
       <c r="E2" t="n">
         <v>70.95110326411077</v>
@@ -516,10 +516,10 @@
         <v>43.00429598386303</v>
       </c>
       <c r="C3" t="n">
-        <v>105.5786320845853</v>
+        <v>98.4204690087752</v>
       </c>
       <c r="D3" t="n">
-        <v>19.18446384412695</v>
+        <v>12.02630076831704</v>
       </c>
       <c r="E3" t="n">
         <v>86.39416824045846</v>
@@ -547,10 +547,10 @@
         <v>38.52737011504853</v>
       </c>
       <c r="C4" t="n">
-        <v>126.2368037973975</v>
+        <v>119.4429166398555</v>
       </c>
       <c r="D4" t="n">
-        <v>19.86431896594604</v>
+        <v>13.07043180840359</v>
       </c>
       <c r="E4" t="n">
         <v>106.3724848314517</v>
@@ -578,10 +578,10 @@
         <v>22.0312137538322</v>
       </c>
       <c r="C5" t="n">
-        <v>30.08627220953744</v>
+        <v>27.89256489766104</v>
       </c>
       <c r="D5" t="n">
-        <v>5.169816518605618</v>
+        <v>2.976109206729212</v>
       </c>
       <c r="E5" t="n">
         <v>24.91645569093177</v>
@@ -609,10 +609,10 @@
         <v>10.71154785150647</v>
       </c>
       <c r="C6" t="n">
-        <v>27.93273264312214</v>
+        <v>25.87783081391243</v>
       </c>
       <c r="D6" t="n">
-        <v>3.691071655728495</v>
+        <v>1.636169826518793</v>
       </c>
       <c r="E6" t="n">
         <v>24.24166098739359</v>
@@ -640,10 +640,10 @@
         <v>73.49010240602721</v>
       </c>
       <c r="C7" t="n">
-        <v>137.778822446604</v>
+        <v>181.8035109186626</v>
       </c>
       <c r="D7" t="n">
-        <v>20.57909690044887</v>
+        <v>64.6037853725084</v>
       </c>
       <c r="E7" t="n">
         <v>117.199725546155</v>
@@ -671,10 +671,10 @@
         <v>38.04800156230241</v>
       </c>
       <c r="C8" t="n">
-        <v>99.34334510048848</v>
+        <v>91.80975688474867</v>
       </c>
       <c r="D8" t="n">
-        <v>25.19954160564174</v>
+        <v>17.66595338990206</v>
       </c>
       <c r="E8" t="n">
         <v>74.14380349484685</v>
@@ -702,10 +702,10 @@
         <v>13.13984742555837</v>
       </c>
       <c r="C9" t="n">
-        <v>23.47635366240364</v>
+        <v>20.52188610557545</v>
       </c>
       <c r="D9" t="n">
-        <v>7.163689626961417</v>
+        <v>4.209222070133255</v>
       </c>
       <c r="E9" t="n">
         <v>16.31266403544219</v>
@@ -733,10 +733,10 @@
         <v>33.67628658821203</v>
       </c>
       <c r="C10" t="n">
-        <v>69.89333986122671</v>
+        <v>62.86138988194384</v>
       </c>
       <c r="D10" t="n">
-        <v>12.30890115368658</v>
+        <v>5.276951174403877</v>
       </c>
       <c r="E10" t="n">
         <v>57.58443870754013</v>
@@ -764,10 +764,10 @@
         <v>34.67685765838427</v>
       </c>
       <c r="C11" t="n">
-        <v>56.55301044801777</v>
+        <v>53.66290083119358</v>
       </c>
       <c r="D11" t="n">
-        <v>11.50492141394462</v>
+        <v>8.614811797120455</v>
       </c>
       <c r="E11" t="n">
         <v>45.04808903407307</v>
@@ -795,10 +795,10 @@
         <v>45.27559719715208</v>
       </c>
       <c r="C12" t="n">
-        <v>95.65478939340061</v>
+        <v>88.37959858545823</v>
       </c>
       <c r="D12" t="n">
-        <v>17.43868450181956</v>
+        <v>10.16349369387679</v>
       </c>
       <c r="E12" t="n">
         <v>78.21610489158107</v>
@@ -826,10 +826,10 @@
         <v>47.53467333448586</v>
       </c>
       <c r="C13" t="n">
-        <v>119.8294371238245</v>
+        <v>109.6919803657956</v>
       </c>
       <c r="D13" t="n">
-        <v>23.27318111152513</v>
+        <v>13.13572435349594</v>
       </c>
       <c r="E13" t="n">
         <v>96.5562560122993</v>
@@ -857,10 +857,10 @@
         <v>35.62198873794238</v>
       </c>
       <c r="C14" t="n">
-        <v>55.34255172678453</v>
+        <v>51.74872726013162</v>
       </c>
       <c r="D14" t="n">
-        <v>10.32615407656282</v>
+        <v>6.732329609910158</v>
       </c>
       <c r="E14" t="n">
         <v>45.01639765022158</v>
@@ -888,10 +888,10 @@
         <v>30.89092109790542</v>
       </c>
       <c r="C15" t="n">
-        <v>49.82780632669913</v>
+        <v>44.88764127486557</v>
       </c>
       <c r="D15" t="n">
-        <v>10.80688710164631</v>
+        <v>5.866722049813027</v>
       </c>
       <c r="E15" t="n">
         <v>39.02091922505266</v>
@@ -919,10 +919,10 @@
         <v>46.97694702763098</v>
       </c>
       <c r="C16" t="n">
-        <v>121.9939643478477</v>
+        <v>114.9389027574633</v>
       </c>
       <c r="D16" t="n">
-        <v>23.18465535842723</v>
+        <v>16.12959376804319</v>
       </c>
       <c r="E16" t="n">
         <v>98.80930898942003</v>
@@ -950,10 +950,10 @@
         <v>32.69564740789706</v>
       </c>
       <c r="C17" t="n">
-        <v>74.14205754793427</v>
+        <v>66.47039923590675</v>
       </c>
       <c r="D17" t="n">
-        <v>15.70790433040031</v>
+        <v>8.036246018373033</v>
       </c>
       <c r="E17" t="n">
         <v>58.43415321753402</v>
@@ -981,10 +981,10 @@
         <v>35.38372528075408</v>
       </c>
       <c r="C18" t="n">
-        <v>69.48005373582909</v>
+        <v>64.98130380093853</v>
       </c>
       <c r="D18" t="n">
-        <v>12.24864212971865</v>
+        <v>7.749892194827897</v>
       </c>
       <c r="E18" t="n">
         <v>57.23141160611062</v>
@@ -1012,10 +1012,10 @@
         <v>28.50233079407887</v>
       </c>
       <c r="C19" t="n">
-        <v>124.8302791164509</v>
+        <v>115.5336202580731</v>
       </c>
       <c r="D19" t="n">
-        <v>16.27367323443209</v>
+        <v>6.977014376054265</v>
       </c>
       <c r="E19" t="n">
         <v>108.5566058820187</v>
@@ -1043,10 +1043,10 @@
         <v>30.79907578112522</v>
       </c>
       <c r="C20" t="n">
-        <v>39.24998239172575</v>
+        <v>36.64975370606664</v>
       </c>
       <c r="D20" t="n">
-        <v>6.734351686518433</v>
+        <v>4.13412300085932</v>
       </c>
       <c r="E20" t="n">
         <v>32.51563070520736</v>
@@ -1074,10 +1074,10 @@
         <v>43.18322830662537</v>
       </c>
       <c r="C21" t="n">
-        <v>40.27660285119649</v>
+        <v>39.70211150743625</v>
       </c>
       <c r="D21" t="n">
-        <v>6.283178926534119</v>
+        <v>5.708687582773737</v>
       </c>
       <c r="E21" t="n">
         <v>33.99342392466239</v>
@@ -1105,10 +1105,10 @@
         <v>13.93478200883266</v>
       </c>
       <c r="C22" t="n">
-        <v>11.40152979038344</v>
+        <v>10.41642217933556</v>
       </c>
       <c r="D22" t="n">
-        <v>2.036011405933333</v>
+        <v>1.05090379488537</v>
       </c>
       <c r="E22" t="n">
         <v>9.365518384450143</v>
@@ -1136,10 +1136,10 @@
         <v>39.10391841843337</v>
       </c>
       <c r="C23" t="n">
-        <v>82.84525216332923</v>
+        <v>73.59300222877866</v>
       </c>
       <c r="D23" t="n">
-        <v>17.71459439340935</v>
+        <v>8.462344458858782</v>
       </c>
       <c r="E23" t="n">
         <v>65.13065776991985</v>
@@ -1167,10 +1167,10 @@
         <v>8.895410527335777</v>
       </c>
       <c r="C24" t="n">
-        <v>7.234749019796491</v>
+        <v>6.272130783095512</v>
       </c>
       <c r="D24" t="n">
-        <v>1.499180814868446</v>
+        <v>0.5365625781674238</v>
       </c>
       <c r="E24" t="n">
         <v>5.735568204928065</v>
@@ -1198,10 +1198,10 @@
         <v>32.15078311540933</v>
       </c>
       <c r="C25" t="n">
-        <v>65.18475180229002</v>
+        <v>58.66873979331869</v>
       </c>
       <c r="D25" t="n">
-        <v>13.87850706010328</v>
+        <v>7.362495051132077</v>
       </c>
       <c r="E25" t="n">
         <v>51.30624474218673</v>
@@ -1229,10 +1229,10 @@
         <v>29.49354862740359</v>
       </c>
       <c r="C26" t="n">
-        <v>71.34631813926337</v>
+        <v>88.37801185544566</v>
       </c>
       <c r="D26" t="n">
-        <v>17.05406743345007</v>
+        <v>34.08576114963231</v>
       </c>
       <c r="E26" t="n">
         <v>54.29225070581326</v>
@@ -1260,10 +1260,10 @@
         <v>23.41695409700751</v>
       </c>
       <c r="C27" t="n">
-        <v>76.66161736134227</v>
+        <v>69.34879879626797</v>
       </c>
       <c r="D27" t="n">
-        <v>20.31908169508977</v>
+        <v>13.0062631300152</v>
       </c>
       <c r="E27" t="n">
         <v>56.34253566625249</v>
@@ -1291,10 +1291,10 @@
         <v>54.79078757173561</v>
       </c>
       <c r="C28" t="n">
-        <v>58.3717185986206</v>
+        <v>55.71036424334256</v>
       </c>
       <c r="D28" t="n">
-        <v>7.179119110806737</v>
+        <v>4.517764755528603</v>
       </c>
       <c r="E28" t="n">
         <v>51.19259948781386</v>
@@ -1322,10 +1322,10 @@
         <v>51.65157223068612</v>
       </c>
       <c r="C29" t="n">
-        <v>196.96674184315</v>
+        <v>190.2666917046467</v>
       </c>
       <c r="D29" t="n">
-        <v>25.12650406213757</v>
+        <v>18.42645392363421</v>
       </c>
       <c r="E29" t="n">
         <v>171.8402377810123</v>
@@ -1353,10 +1353,10 @@
         <v>33.23192080432319</v>
       </c>
       <c r="C30" t="n">
-        <v>68.99726735364825</v>
+        <v>63.22384352504145</v>
       </c>
       <c r="D30" t="n">
-        <v>13.27110586746939</v>
+        <v>7.497682038862504</v>
       </c>
       <c r="E30" t="n">
         <v>55.72616148617894</v>
@@ -1384,10 +1384,10 @@
         <v>10.13161505062967</v>
       </c>
       <c r="C31" t="n">
-        <v>71.14167134139169</v>
+        <v>69.8647025646125</v>
       </c>
       <c r="D31" t="n">
-        <v>8.338862063791087</v>
+        <v>7.061893287011926</v>
       </c>
       <c r="E31" t="n">
         <v>62.80280927760071</v>
@@ -1415,10 +1415,10 @@
         <v>13.80881345161295</v>
       </c>
       <c r="C32" t="n">
-        <v>20.08465027070292</v>
+        <v>17.49108955688107</v>
       </c>
       <c r="D32" t="n">
-        <v>4.489027332171283</v>
+        <v>1.895466618349366</v>
       </c>
       <c r="E32" t="n">
         <v>15.59562293853169</v>
@@ -1446,10 +1446,10 @@
         <v>32.36077714132275</v>
       </c>
       <c r="C33" t="n">
-        <v>107.8838396743842</v>
+        <v>99.52386531570954</v>
       </c>
       <c r="D33" t="n">
-        <v>18.82406307980375</v>
+        <v>10.46408872112913</v>
       </c>
       <c r="E33" t="n">
         <v>89.05977659458009</v>
@@ -1477,10 +1477,10 @@
         <v>38.99438134435925</v>
       </c>
       <c r="C34" t="n">
-        <v>151.9907538482498</v>
+        <v>145.7929087768983</v>
       </c>
       <c r="D34" t="n">
-        <v>26.25849816336722</v>
+        <v>20.06065309201589</v>
       </c>
       <c r="E34" t="n">
         <v>125.7322556848826</v>
@@ -1508,10 +1508,10 @@
         <v>24.92726987785904</v>
       </c>
       <c r="C35" t="n">
-        <v>44.07745611946676</v>
+        <v>43.96739964255068</v>
       </c>
       <c r="D35" t="n">
-        <v>4.8906918335445</v>
+        <v>4.780635356628347</v>
       </c>
       <c r="E35" t="n">
         <v>39.18676428592234</v>
@@ -1539,10 +1539,10 @@
         <v>22.5815483367999</v>
       </c>
       <c r="C36" t="n">
-        <v>50.123356302476</v>
+        <v>45.53085768534857</v>
       </c>
       <c r="D36" t="n">
-        <v>9.874081691963982</v>
+        <v>5.281583074836819</v>
       </c>
       <c r="E36" t="n">
         <v>40.2492746105118</v>
@@ -1570,10 +1570,10 @@
         <v>27.89941322511557</v>
       </c>
       <c r="C37" t="n">
-        <v>20.99807058750797</v>
+        <v>19.65123610670828</v>
       </c>
       <c r="D37" t="n">
-        <v>3.731273854353825</v>
+        <v>2.384439373554106</v>
       </c>
       <c r="E37" t="n">
         <v>17.26679673315413</v>
@@ -1601,10 +1601,10 @@
         <v>49.13405460207678</v>
       </c>
       <c r="C38" t="n">
-        <v>46.85031021693825</v>
+        <v>45.10051721391826</v>
       </c>
       <c r="D38" t="n">
-        <v>5.6075239477809</v>
+        <v>3.857730944760764</v>
       </c>
       <c r="E38" t="n">
         <v>41.24278626915751</v>
@@ -1632,10 +1632,10 @@
         <v>41.05150043132295</v>
       </c>
       <c r="C39" t="n">
-        <v>92.75111705271379</v>
+        <v>87.07867503560531</v>
       </c>
       <c r="D39" t="n">
-        <v>16.7800852887136</v>
+        <v>11.10764327160515</v>
       </c>
       <c r="E39" t="n">
         <v>75.97103176400019</v>
@@ -1663,10 +1663,10 @@
         <v>38.98198825898191</v>
       </c>
       <c r="C40" t="n">
-        <v>53.21516247643582</v>
+        <v>48.08977013335183</v>
       </c>
       <c r="D40" t="n">
-        <v>10.65632961466042</v>
+        <v>5.530937271576509</v>
       </c>
       <c r="E40" t="n">
         <v>42.55883286177546</v>
@@ -1694,10 +1694,10 @@
         <v>21.53316810965194</v>
       </c>
       <c r="C41" t="n">
-        <v>48.93494326358779</v>
+        <v>48.00476824953135</v>
       </c>
       <c r="D41" t="n">
-        <v>7.521858064216178</v>
+        <v>6.591683050160187</v>
       </c>
       <c r="E41" t="n">
         <v>41.41308519937129</v>
@@ -1725,10 +1725,10 @@
         <v>11.42757655397756</v>
       </c>
       <c r="C42" t="n">
-        <v>32.74568226853118</v>
+        <v>32.09902297667693</v>
       </c>
       <c r="D42" t="n">
-        <v>4.105690768775577</v>
+        <v>3.459031476921247</v>
       </c>
       <c r="E42" t="n">
         <v>28.63999149975572</v>
@@ -1756,10 +1756,10 @@
         <v>23.01598922829499</v>
       </c>
       <c r="C43" t="n">
-        <v>70.66149189660931</v>
+        <v>67.04340374934132</v>
       </c>
       <c r="D43" t="n">
-        <v>7.681560900135334</v>
+        <v>4.063472752867128</v>
       </c>
       <c r="E43" t="n">
         <v>62.97993099647422</v>
@@ -1787,10 +1787,10 @@
         <v>87.1553790019391</v>
       </c>
       <c r="C44" t="n">
-        <v>116.1648819044016</v>
+        <v>105.3052184104982</v>
       </c>
       <c r="D44" t="n">
-        <v>23.08395505065983</v>
+        <v>12.22429155675636</v>
       </c>
       <c r="E44" t="n">
         <v>93.08092685374159</v>
@@ -1818,10 +1818,10 @@
         <v>9.429887758464357</v>
       </c>
       <c r="C45" t="n">
-        <v>14.30848021196943</v>
+        <v>12.84495941074148</v>
       </c>
       <c r="D45" t="n">
-        <v>3.228969748135051</v>
+        <v>1.765448946907162</v>
       </c>
       <c r="E45" t="n">
         <v>11.07951046383434</v>
@@ -1849,10 +1849,10 @@
         <v>20.68266150165245</v>
       </c>
       <c r="C46" t="n">
-        <v>28.20536135887886</v>
+        <v>27.85905107255654</v>
       </c>
       <c r="D46" t="n">
-        <v>1.971881552763135</v>
+        <v>1.625571266440792</v>
       </c>
       <c r="E46" t="n">
         <v>26.23347980611576</v>
@@ -1880,10 +1880,10 @@
         <v>12.29824065136684</v>
       </c>
       <c r="C47" t="n">
-        <v>4.971515574622869</v>
+        <v>4.607196448654674</v>
       </c>
       <c r="D47" t="n">
-        <v>0.8886826245007255</v>
+        <v>0.5243634985325216</v>
       </c>
       <c r="E47" t="n">
         <v>4.082832950122159</v>
@@ -1911,10 +1911,10 @@
         <v>13.03741085203557</v>
       </c>
       <c r="C48" t="n">
-        <v>28.37055141351259</v>
+        <v>26.62102564419216</v>
       </c>
       <c r="D48" t="n">
-        <v>4.441164344526591</v>
+        <v>2.691638575206132</v>
       </c>
       <c r="E48" t="n">
         <v>23.92938706898602</v>
@@ -1942,10 +1942,10 @@
         <v>22.09889380777077</v>
       </c>
       <c r="C49" t="n">
-        <v>36.96450900202955</v>
+        <v>33.38746513947333</v>
       </c>
       <c r="D49" t="n">
-        <v>7.487232119632741</v>
+        <v>3.91018825707657</v>
       </c>
       <c r="E49" t="n">
         <v>29.4772768823968</v>
@@ -1973,10 +1973,10 @@
         <v>20.74357099544427</v>
       </c>
       <c r="C50" t="n">
-        <v>27.06981267115147</v>
+        <v>25.44325883016047</v>
       </c>
       <c r="D50" t="n">
-        <v>3.612902888003783</v>
+        <v>1.986349047012836</v>
       </c>
       <c r="E50" t="n">
         <v>23.45690978314757</v>

</xml_diff>